<commit_message>
update mot so cai
</commit_message>
<xml_diff>
--- a/QLyBanVatTu/GUI/bin/Debug/DanhSachDonHang.xlsx
+++ b/QLyBanVatTu/GUI/bin/Debug/DanhSachDonHang.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet 1" sheetId="1" r:id="Rbbd989ed3fcf4c34"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet 1" sheetId="1" r:id="R8711b3e614e54071"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -32,47 +32,7 @@
     </x:row>
     <x:row>
       <x:c t="str">
-        <x:v>HDX01</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>Trần Thị B</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>456 Đường XYZ, Quận 2, TP. HCM</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>123456789</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>4/8/2023 12:00:00 AM</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row>
-      <x:c t="str">
-        <x:v>HDX2</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>Trần Thị B</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>456 Đường XYZ, Quận 2, TP. HCM</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>123456789</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>4/8/2023 12:00:00 AM</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row>
-      <x:c t="str">
-        <x:v>HDX3</x:v>
+        <x:v>HDX_7</x:v>
       </x:c>
       <x:c t="str">
         <x:v>Nguyễn Văn A</x:v>
@@ -84,50 +44,30 @@
         <x:v>123456789</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>4/8/2023 12:00:00 AM</x:v>
+        <x:v>4/9/2023 12:00:00 AM</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>131111</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row>
       <x:c t="str">
-        <x:v>HDX4</x:v>
+        <x:v>HDX_8</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>cu Ân</x:v>
+        <x:v>Nguyễn Văn A</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>fsdfsdfsdfsf</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>942343242</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>4/8/2023 12:00:00 AM</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>1111</x:v>
-      </x:c>
-    </x:row>
-    <x:row>
-      <x:c t="str">
-        <x:v>HDX5</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>Trần Thị B</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>456 Đường XYZ, Quận 2, TP. HCM</x:v>
+        <x:v>123 Đường ABC, Quận 1, TP. HCM</x:v>
       </x:c>
       <x:c t="n">
         <x:v>123456789</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>4/8/2023 12:00:00 AM</x:v>
+        <x:v>4/9/2023 12:00:00 AM</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>120000</x:v>
+        <x:v>52000</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -152,10 +92,10 @@
     </x:row>
     <x:row>
       <x:c t="str">
-        <x:v>Doanh thu 2023-04-08 -&gt; 2023-04-08</x:v>
+        <x:v>Doanh thu 2023-04-08 -&gt; 2023-04-29</x:v>
       </x:c>
       <x:c t="n">
-        <x:v>252222</x:v>
+        <x:v>52000</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>